<commit_message>
images and tracking file
</commit_message>
<xml_diff>
--- a/contents/art_submissions/submission_tracking.xlsx
+++ b/contents/art_submissions/submission_tracking.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wzhang/Documents/Personal/verazhang/contents/art_submissions/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{DCC0B0C7-3493-7E49-BCFF-818ED31E009F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35BF4BD7-F8C5-0641-AC2B-DD448A6158B0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2780" yWindow="1560" windowWidth="28040" windowHeight="17440" xr2:uid="{5D8B7C3F-8132-D049-A181-2560E76CB836}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="39">
   <si>
     <t>https://www.artistaday.com</t>
   </si>
@@ -48,6 +48,105 @@
   </si>
   <si>
     <t>Response</t>
+  </si>
+  <si>
+    <t>Source</t>
+  </si>
+  <si>
+    <t>https://www.lightspacetime.art/30-art-websites-accepting-free-art-submissions-from-artists/</t>
+  </si>
+  <si>
+    <t>https://www.thisiscolossal.com/submissions/</t>
+  </si>
+  <si>
+    <t>https://mymodernmet.com/</t>
+  </si>
+  <si>
+    <t>No.</t>
+  </si>
+  <si>
+    <t>NO</t>
+  </si>
+  <si>
+    <t>https://www.tusslemagazine.com/about-us</t>
+  </si>
+  <si>
+    <t>https://www.ignant.com/submissions</t>
+  </si>
+  <si>
+    <t>https://picdit.net/submit</t>
+  </si>
+  <si>
+    <t>http://www.crossconnectmag.com/submit</t>
+  </si>
+  <si>
+    <t>http://www.emptykingdom.com/submit</t>
+  </si>
+  <si>
+    <t>http://www.ufunk.net/en/submit</t>
+  </si>
+  <si>
+    <t>http://eatsleepdraw.com/submit</t>
+  </si>
+  <si>
+    <t>http://theyouth-.tumblr.com/submit</t>
+  </si>
+  <si>
+    <t>http://emptyeasel.com/artwork-submission-form</t>
+  </si>
+  <si>
+    <t>http://just-art.tumblr.com/submit</t>
+  </si>
+  <si>
+    <t>https://issuu.com/artnois</t>
+  </si>
+  <si>
+    <t>http://www.artandbeyondpublications.com/magazine-entry</t>
+  </si>
+  <si>
+    <t>http://www.artrevealmagazine.com/submission</t>
+  </si>
+  <si>
+    <t>http://nonsensesociety.com</t>
+  </si>
+  <si>
+    <t>https://digitalartlive.com/get-published</t>
+  </si>
+  <si>
+    <t>https://issuu.com/bunburymagazine</t>
+  </si>
+  <si>
+    <t>http://www.creativefluff.com/submit-articles</t>
+  </si>
+  <si>
+    <t>http://artistsinspireartists.com/submit-art-submissions</t>
+  </si>
+  <si>
+    <t>http://www.jazjaz.net/submit-your-art-2</t>
+  </si>
+  <si>
+    <t>http://www.dailyartfixx.com/submissions</t>
+  </si>
+  <si>
+    <t>http://supersonicart.com/submit-your-art</t>
+  </si>
+  <si>
+    <t>https://www.pantamagazine.com/collaborate</t>
+  </si>
+  <si>
+    <t>http://theartelephant.com/work-with-tae-2</t>
+  </si>
+  <si>
+    <t>http://www.peopleofprint.com/submit</t>
+  </si>
+  <si>
+    <t>http://insideartists.co.uk/features.html</t>
+  </si>
+  <si>
+    <t>http://forgeartmag.com/submit</t>
+  </si>
+  <si>
+    <t>https://superiormagazine.submittable.com/submit</t>
   </si>
 </sst>
 </file>
@@ -92,9 +191,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -410,42 +512,404 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{53D815D4-0C07-F44E-B9FF-3FDE585B6E05}">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:E32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="24.83203125" customWidth="1"/>
+    <col min="1" max="1" width="10.83203125" style="2"/>
+    <col min="2" max="2" width="42.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" t="s">
         <v>1</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C2" t="s">
         <v>2</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D2" t="s">
         <v>3</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" s="2">
+        <v>1</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C3" t="s">
         <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" s="2">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" s="2">
+        <v>3</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" s="2">
+        <v>4</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" s="2">
+        <v>5</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" s="2">
+        <v>6</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" s="2">
+        <v>7</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C9" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" s="2">
+        <v>8</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C10" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11" s="2">
+        <v>9</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C11" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12" s="2">
+        <v>10</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C12" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13" s="2">
+        <v>11</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C13" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14" s="2">
+        <v>12</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C14" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A15" s="2">
+        <v>13</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C15" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A16" s="2">
+        <v>14</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C16" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17" s="2">
+        <v>15</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C17" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A18" s="2">
+        <v>16</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C18" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A19" s="2">
+        <v>17</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C19" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A20" s="2">
+        <v>18</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C20" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A21" s="2">
+        <v>19</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C21" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A22" s="2">
+        <v>20</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C22" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A23" s="2">
+        <v>21</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C23" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A24" s="2">
+        <v>22</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C24" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A25" s="2">
+        <v>23</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C25" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A26" s="2">
+        <v>24</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C26" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A27" s="2">
+        <v>25</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C27" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A28" s="2">
+        <v>26</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C28" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A29" s="2">
+        <v>27</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C29" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A30" s="2">
+        <v>28</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C30" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A31" s="2">
+        <v>29</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C31" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A32" s="2">
+        <v>30</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C32" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="https://www.artistaday.com/" xr:uid="{5FA140C4-3166-CE41-B5FC-2878A0924FC3}"/>
+    <hyperlink ref="B3" r:id="rId1" display="https://www.artistaday.com/" xr:uid="{5FA140C4-3166-CE41-B5FC-2878A0924FC3}"/>
+    <hyperlink ref="B5" r:id="rId2" xr:uid="{8761972E-7FC3-8C4C-A543-C88A05ABE818}"/>
+    <hyperlink ref="B6" r:id="rId3" xr:uid="{0FEAA4C0-3539-A94F-BF22-B0946F2D16EA}"/>
+    <hyperlink ref="B7" r:id="rId4" display="https://www.ignant.com/submissions/" xr:uid="{84EA8C54-9C6B-C147-82FF-7C894914C37C}"/>
+    <hyperlink ref="B8" r:id="rId5" display="https://picdit.net/submit/" xr:uid="{BD6095B5-98FF-164C-9CF2-CB05635C5CCA}"/>
+    <hyperlink ref="B9" r:id="rId6" xr:uid="{34EAF5F3-51F9-6E48-A250-C0560C74E772}"/>
+    <hyperlink ref="B10" r:id="rId7" display="http://www.emptykingdom.com/submit/" xr:uid="{77351D87-8F8C-6E44-8013-7D805E9D5F9C}"/>
+    <hyperlink ref="B11" r:id="rId8" display="http://www.ufunk.net/en/submit/" xr:uid="{3BF950C3-40CA-1044-B546-C40E4837CDF3}"/>
+    <hyperlink ref="B12" r:id="rId9" xr:uid="{6E6B3740-BB78-944B-AB75-BD3BB768D5D9}"/>
+    <hyperlink ref="B13" r:id="rId10" xr:uid="{118A401C-AFE3-8147-A6AB-6BC480CE00ED}"/>
+    <hyperlink ref="B14" r:id="rId11" display="http://emptyeasel.com/artwork-submission-form/" xr:uid="{99D1C319-DF8D-5C41-890A-E29A5D3BDE7C}"/>
+    <hyperlink ref="B15" r:id="rId12" xr:uid="{E49C3EC3-D7DF-EA44-B0BD-18F4880775A5}"/>
+    <hyperlink ref="B16" r:id="rId13" xr:uid="{2B73629D-4921-3C47-90DF-4EC2F1BB73E4}"/>
+    <hyperlink ref="B17" r:id="rId14" display="http://www.artandbeyondpublications.com/magazine-entry/" xr:uid="{5E903289-5518-704A-B456-09D0A3E7FEAD}"/>
+    <hyperlink ref="B18" r:id="rId15" display="http://www.artrevealmagazine.com/submission/" xr:uid="{A468BF6B-4B76-964F-85FA-CB3FFBBBB91A}"/>
+    <hyperlink ref="B19" r:id="rId16" display="http://nonsensesociety.com/" xr:uid="{25CA2EDB-A57D-384F-9925-DB67B41FB19B}"/>
+    <hyperlink ref="B20" r:id="rId17" display="https://digitalartlive.com/get-published/" xr:uid="{FD0C94E7-ED69-D14B-890E-C58CBC8B1D2B}"/>
+    <hyperlink ref="B21" r:id="rId18" xr:uid="{C3E759A1-3CCA-C64D-9DD5-19CB5FF1CBA5}"/>
+    <hyperlink ref="B22" r:id="rId19" display="http://www.creativefluff.com/submit-articles/" xr:uid="{376DDEF9-4144-2D41-98C7-28E28C204FC2}"/>
+    <hyperlink ref="B23" r:id="rId20" xr:uid="{4891C020-76C3-B54A-B2A0-1F15A4F17CD4}"/>
+    <hyperlink ref="B24" r:id="rId21" xr:uid="{7D22083C-79BF-3A4B-A45C-54B27F8A2B0A}"/>
+    <hyperlink ref="B25" r:id="rId22" display="http://www.dailyartfixx.com/submissions/" xr:uid="{6DD06C06-67B4-5D43-BBA4-5A56386C2FD6}"/>
+    <hyperlink ref="B26" r:id="rId23" xr:uid="{2929E351-FF40-9E48-B951-A813F4BF0D61}"/>
+    <hyperlink ref="B27" r:id="rId24" display="https://www.pantamagazine.com/collaborate/" xr:uid="{C3396B84-FDA1-1541-BF82-4CA9B16A8F6B}"/>
+    <hyperlink ref="B28" r:id="rId25" xr:uid="{7C90A12F-E494-954C-A25B-A580660749F6}"/>
+    <hyperlink ref="B29" r:id="rId26" display="http://www.peopleofprint.com/submit/" xr:uid="{3E674F10-861A-6D4F-BA6C-ACA419D58137}"/>
+    <hyperlink ref="B30" r:id="rId27" xr:uid="{B1CF945E-DA5A-9A4A-A186-397C85F5DF3D}"/>
+    <hyperlink ref="B31" r:id="rId28" xr:uid="{5085346D-8749-7143-82E7-930B9BEB487A}"/>
+    <hyperlink ref="B32" r:id="rId29" xr:uid="{4B0C4570-0178-EA47-B0D9-6FA851CB065A}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>